<commit_message>
hmm, maybe this will work?
</commit_message>
<xml_diff>
--- a/tests/testthat/merge_test.xlsx
+++ b/tests/testthat/merge_test.xlsx
@@ -94,8 +94,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -109,9 +111,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,7 +448,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
going back, trying to find out why travis acts weird
</commit_message>
<xml_diff>
--- a/tests/testthat/merge_test.xlsx
+++ b/tests/testthat/merge_test.xlsx
@@ -94,10 +94,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -111,11 +109,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,7 +444,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>